<commit_message>
this version is working as desired
</commit_message>
<xml_diff>
--- a/Second Model/keywords list.xlsx
+++ b/Second Model/keywords list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Python/Analysis/2024/AdjustCreditLogs/PX2_AdjustCredit_Log/Second Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91F899C4-08B2-7143-A2EE-8F94B01C0C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8CC18A-3F28-0447-8D85-2EC395326B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="740" windowWidth="28100" windowHeight="17260" xr2:uid="{8784EA1A-6346-384F-A7B2-34A387578430}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>get network status:</t>
   </si>
   <si>
-    <t>bat_monitor:</t>
-  </si>
-  <si>
     <t>Signal quality:</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t xml:space="preserve">aws_Connect : </t>
   </si>
   <si>
-    <t>[14:15:29.275] INFO: bat_monitor: vol:3559.47 state 2</t>
-  </si>
-  <si>
     <t>[14:16:15.464] INFO: pppos_new: get network status: type=0, stat=5</t>
   </si>
   <si>
@@ -219,6 +213,12 @@
   </si>
   <si>
     <t xml:space="preserve">Value </t>
+  </si>
+  <si>
+    <t>cpu_start:</t>
+  </si>
+  <si>
+    <t>[11:39:21.922]IN¡û¡ô_x001B_[0;32mI (92) cpu_start: Pro cpu start user code_x001B_</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="C1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:E22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,21 +615,21 @@
   <sheetData>
     <row r="1" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.2">
@@ -640,7 +640,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="2">
         <v>2429999004</v>
@@ -654,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F4" s="2">
         <v>8.9457300000022004E+19</v>
@@ -682,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
@@ -696,7 +696,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>12</v>
@@ -707,7 +707,7 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>11</v>
@@ -715,15 +715,15 @@
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>26</v>
@@ -731,10 +731,10 @@
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -745,7 +745,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
@@ -753,10 +753,10 @@
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
@@ -764,10 +764,10 @@
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -775,10 +775,10 @@
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
@@ -786,10 +786,10 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
@@ -797,10 +797,10 @@
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
@@ -808,10 +808,10 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
         <v>22</v>
@@ -819,10 +819,10 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
         <v>23</v>
@@ -830,10 +830,10 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
@@ -841,10 +841,10 @@
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>

</xml_diff>